<commit_message>
Fixed up folder structure
</commit_message>
<xml_diff>
--- a/data/grid_search_xl.xlsx
+++ b/data/grid_search_xl.xlsx
@@ -8,13 +8,28 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Iva Wright\Documents\engineering-2024-sem2\ENGSCI700B\p4p\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{AB9BC503-3233-4BDB-835A-5B0AB148BEAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44D68ABD-8440-4514-968C-865C4606F572}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1C994122-426C-4E31-9AF6-B67E56D1AC14}"/>
   </bookViews>
   <sheets>
     <sheet name="grid_search" sheetId="1" r:id="rId1"/>
+    <sheet name="Epochs" sheetId="2" r:id="rId2"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlchart.v1.0" hidden="1">Epochs!$E$2</definedName>
+    <definedName name="_xlchart.v1.1" hidden="1">Epochs!$E$3</definedName>
+    <definedName name="_xlchart.v1.10" hidden="1">Epochs!$F$3</definedName>
+    <definedName name="_xlchart.v1.11" hidden="1">Epochs!$F$3:$F$146</definedName>
+    <definedName name="_xlchart.v1.2" hidden="1">Epochs!$E$3:$E$146</definedName>
+    <definedName name="_xlchart.v1.3" hidden="1">Epochs!$F$2</definedName>
+    <definedName name="_xlchart.v1.4" hidden="1">Epochs!$F$3</definedName>
+    <definedName name="_xlchart.v1.5" hidden="1">Epochs!$F$3:$F$146</definedName>
+    <definedName name="_xlchart.v1.6" hidden="1">Epochs!$E$2</definedName>
+    <definedName name="_xlchart.v1.7" hidden="1">Epochs!$E$3</definedName>
+    <definedName name="_xlchart.v1.8" hidden="1">Epochs!$E$3:$E$146</definedName>
+    <definedName name="_xlchart.v1.9" hidden="1">Epochs!$F$2</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <fileRecoveryPr repairLoad="1"/>
   <extLst>
@@ -31,6 +46,28 @@
     </ext>
   </extLst>
 </workbook>
+</file>
+
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1059,13 +1096,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{83D6D337-6E05-40ED-9BE6-404CA955A007}">
   <dimension ref="B2:O146"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A81" workbookViewId="0">
-      <selection activeCell="E115" sqref="E115"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="4" max="4" width="11.88671875" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="24.44140625" customWidth="1"/>
     <col min="12" max="12" width="31.6640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="11.21875" bestFit="1" customWidth="1"/>
   </cols>
@@ -5447,4 +5486,2509 @@
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12CFA855-D564-423C-9809-E3B49D58B336}">
+  <dimension ref="B2:I146"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="2" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B2" cm="1">
+        <f t="array" ref="B2:F146">grid_search!B2:'grid_search'!F146</f>
+        <v>0</v>
+      </c>
+      <c r="C2" t="str">
+        <v>Model</v>
+      </c>
+      <c r="D2" t="str">
+        <v>Learning Rate</v>
+      </c>
+      <c r="E2" t="str">
+        <v>MSE</v>
+      </c>
+      <c r="F2" t="str">
+        <v>Num. Epochs</v>
+      </c>
+    </row>
+    <row r="3" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B3">
+        <v>0</v>
+      </c>
+      <c r="C3" t="str">
+        <v>seq_model</v>
+      </c>
+      <c r="D3">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E3">
+        <v>1.2016484309382999E-2</v>
+      </c>
+      <c r="F3">
+        <v>8</v>
+      </c>
+      <c r="H3">
+        <f>SUMIF($F$3:$F$146,8,$E$3:$E$146)</f>
+        <v>1.3679521497970382</v>
+      </c>
+      <c r="I3">
+        <f>H3/144</f>
+        <v>9.4996677069238769E-3</v>
+      </c>
+    </row>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B4">
+        <v>1</v>
+      </c>
+      <c r="C4" t="str">
+        <v>seq_model</v>
+      </c>
+      <c r="D4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E4">
+        <v>1.2345075343304399E-2</v>
+      </c>
+      <c r="F4">
+        <v>10</v>
+      </c>
+      <c r="H4">
+        <f>SUMIF($F$3:$F$146,10,$E$3:$E$146)</f>
+        <v>1.1205427747284125</v>
+      </c>
+      <c r="I4">
+        <f t="shared" ref="I4:I5" si="0">H4/144</f>
+        <v>7.7815470467250862E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5" t="str">
+        <v>seq_model</v>
+      </c>
+      <c r="D5">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E5">
+        <v>1.23980222745951E-2</v>
+      </c>
+      <c r="F5">
+        <v>14</v>
+      </c>
+      <c r="H5">
+        <f>SUMIF($F$3:$F$146,14,$E$3:$E$146)</f>
+        <v>0.97232909141642132</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="0"/>
+        <v>6.7522853570584811E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="str">
+        <v>seq_model</v>
+      </c>
+      <c r="D6">
+        <v>1E-3</v>
+      </c>
+      <c r="E6">
+        <v>1.46819067188647E-2</v>
+      </c>
+      <c r="F6">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B7">
+        <v>4</v>
+      </c>
+      <c r="C7" t="str">
+        <v>seq_model</v>
+      </c>
+      <c r="D7">
+        <v>1E-3</v>
+      </c>
+      <c r="E7">
+        <v>1.44573376425588E-2</v>
+      </c>
+      <c r="F7">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B8">
+        <v>5</v>
+      </c>
+      <c r="C8" t="str">
+        <v>seq_model</v>
+      </c>
+      <c r="D8">
+        <v>1E-3</v>
+      </c>
+      <c r="E8">
+        <v>1.3963998870053999E-2</v>
+      </c>
+      <c r="F8">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B9">
+        <v>6</v>
+      </c>
+      <c r="C9" t="str">
+        <v>seq_model</v>
+      </c>
+      <c r="D9">
+        <v>1E-4</v>
+      </c>
+      <c r="E9">
+        <v>0.125644242173307</v>
+      </c>
+      <c r="F9">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B10">
+        <v>7</v>
+      </c>
+      <c r="C10" t="str">
+        <v>seq_model</v>
+      </c>
+      <c r="D10">
+        <v>1E-4</v>
+      </c>
+      <c r="E10">
+        <v>7.9126970225698104E-2</v>
+      </c>
+      <c r="F10">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11" t="str">
+        <v>seq_model</v>
+      </c>
+      <c r="D11">
+        <v>1E-4</v>
+      </c>
+      <c r="E11">
+        <v>2.4651631148449499E-2</v>
+      </c>
+      <c r="F11">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B12">
+        <v>9</v>
+      </c>
+      <c r="C12" t="str">
+        <v>create_custom_model</v>
+      </c>
+      <c r="D12">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E12">
+        <v>1.2896105001614399E-2</v>
+      </c>
+      <c r="F12">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="str">
+        <v>create_custom_model</v>
+      </c>
+      <c r="D13">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E13">
+        <v>1.38821153362579E-2</v>
+      </c>
+      <c r="F13">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B14">
+        <v>11</v>
+      </c>
+      <c r="C14" t="str">
+        <v>create_custom_model</v>
+      </c>
+      <c r="D14">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E14">
+        <v>1.33149809326233E-2</v>
+      </c>
+      <c r="F14">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B15">
+        <v>12</v>
+      </c>
+      <c r="C15" t="str">
+        <v>create_custom_model</v>
+      </c>
+      <c r="D15">
+        <v>1E-3</v>
+      </c>
+      <c r="E15">
+        <v>1.4570422231832299E-2</v>
+      </c>
+      <c r="F15">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="B16">
+        <v>13</v>
+      </c>
+      <c r="C16" t="str">
+        <v>create_custom_model</v>
+      </c>
+      <c r="D16">
+        <v>1E-3</v>
+      </c>
+      <c r="E16">
+        <v>1.4324061268477699E-2</v>
+      </c>
+      <c r="F16">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B17">
+        <v>14</v>
+      </c>
+      <c r="C17" t="str">
+        <v>create_custom_model</v>
+      </c>
+      <c r="D17">
+        <v>1E-3</v>
+      </c>
+      <c r="E17">
+        <v>1.41209929466626E-2</v>
+      </c>
+      <c r="F17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B18">
+        <v>15</v>
+      </c>
+      <c r="C18" t="str">
+        <v>create_custom_model</v>
+      </c>
+      <c r="D18">
+        <v>1E-4</v>
+      </c>
+      <c r="E18">
+        <v>2.1113251115022599E-2</v>
+      </c>
+      <c r="F18">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B19">
+        <v>16</v>
+      </c>
+      <c r="C19" t="str">
+        <v>create_custom_model</v>
+      </c>
+      <c r="D19">
+        <v>1E-4</v>
+      </c>
+      <c r="E19">
+        <v>1.8343751629045699E-2</v>
+      </c>
+      <c r="F19">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B20">
+        <v>17</v>
+      </c>
+      <c r="C20" t="str">
+        <v>create_custom_model</v>
+      </c>
+      <c r="D20">
+        <v>1E-4</v>
+      </c>
+      <c r="E20">
+        <v>1.76720482248457E-2</v>
+      </c>
+      <c r="F20">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B21">
+        <v>18</v>
+      </c>
+      <c r="C21" t="str">
+        <v>single_lstm_dense_output</v>
+      </c>
+      <c r="D21">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E21">
+        <v>1.23586176585128E-2</v>
+      </c>
+      <c r="F21">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B22">
+        <v>19</v>
+      </c>
+      <c r="C22" t="str">
+        <v>single_lstm_dense_output</v>
+      </c>
+      <c r="D22">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E22">
+        <v>1.25378011782428E-2</v>
+      </c>
+      <c r="F22">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B23">
+        <v>20</v>
+      </c>
+      <c r="C23" t="str">
+        <v>single_lstm_dense_output</v>
+      </c>
+      <c r="D23">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E23">
+        <v>1.25919458867887E-2</v>
+      </c>
+      <c r="F23">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B24">
+        <v>21</v>
+      </c>
+      <c r="C24" t="str">
+        <v>single_lstm_dense_output</v>
+      </c>
+      <c r="D24">
+        <v>1E-3</v>
+      </c>
+      <c r="E24">
+        <v>1.37996686309128E-2</v>
+      </c>
+      <c r="F24">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B25">
+        <v>22</v>
+      </c>
+      <c r="C25" t="str">
+        <v>single_lstm_dense_output</v>
+      </c>
+      <c r="D25">
+        <v>1E-3</v>
+      </c>
+      <c r="E25">
+        <v>1.40280371672587E-2</v>
+      </c>
+      <c r="F25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26">
+        <v>23</v>
+      </c>
+      <c r="C26" t="str">
+        <v>single_lstm_dense_output</v>
+      </c>
+      <c r="D26">
+        <v>1E-3</v>
+      </c>
+      <c r="E26">
+        <v>1.40360203339586E-2</v>
+      </c>
+      <c r="F26">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B27">
+        <v>24</v>
+      </c>
+      <c r="C27" t="str">
+        <v>single_lstm_dense_output</v>
+      </c>
+      <c r="D27">
+        <v>1E-4</v>
+      </c>
+      <c r="E27">
+        <v>7.8217735505063696E-2</v>
+      </c>
+      <c r="F27">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B28">
+        <v>25</v>
+      </c>
+      <c r="C28" t="str">
+        <v>single_lstm_dense_output</v>
+      </c>
+      <c r="D28">
+        <v>1E-4</v>
+      </c>
+      <c r="E28">
+        <v>6.3785415528315098E-2</v>
+      </c>
+      <c r="F28">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B29">
+        <v>26</v>
+      </c>
+      <c r="C29" t="str">
+        <v>single_lstm_dense_output</v>
+      </c>
+      <c r="D29">
+        <v>1E-4</v>
+      </c>
+      <c r="E29">
+        <v>3.0135156583737398E-2</v>
+      </c>
+      <c r="F29">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B30">
+        <v>27</v>
+      </c>
+      <c r="C30" t="str">
+        <v>two_layer_lstm</v>
+      </c>
+      <c r="D30">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E30">
+        <v>1.3525713037244799E-2</v>
+      </c>
+      <c r="F30">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B31">
+        <v>28</v>
+      </c>
+      <c r="C31" t="str">
+        <v>two_layer_lstm</v>
+      </c>
+      <c r="D31">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E31">
+        <v>1.25747834593873E-2</v>
+      </c>
+      <c r="F31">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B32">
+        <v>29</v>
+      </c>
+      <c r="C32" t="str">
+        <v>two_layer_lstm</v>
+      </c>
+      <c r="D32">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E32">
+        <v>1.29036815216741E-2</v>
+      </c>
+      <c r="F32">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <v>30</v>
+      </c>
+      <c r="C33" t="str">
+        <v>two_layer_lstm</v>
+      </c>
+      <c r="D33">
+        <v>1E-3</v>
+      </c>
+      <c r="E33">
+        <v>1.4389214569094699E-2</v>
+      </c>
+      <c r="F33">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <v>31</v>
+      </c>
+      <c r="C34" t="str">
+        <v>two_layer_lstm</v>
+      </c>
+      <c r="D34">
+        <v>1E-3</v>
+      </c>
+      <c r="E34">
+        <v>1.4313174811530801E-2</v>
+      </c>
+      <c r="F34">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B35">
+        <v>32</v>
+      </c>
+      <c r="C35" t="str">
+        <v>two_layer_lstm</v>
+      </c>
+      <c r="D35">
+        <v>1E-3</v>
+      </c>
+      <c r="E35">
+        <v>1.3805968370571801E-2</v>
+      </c>
+      <c r="F35">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B36">
+        <v>33</v>
+      </c>
+      <c r="C36" t="str">
+        <v>two_layer_lstm</v>
+      </c>
+      <c r="D36">
+        <v>1E-4</v>
+      </c>
+      <c r="E36">
+        <v>2.5515149214397001E-2</v>
+      </c>
+      <c r="F36">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B37">
+        <v>34</v>
+      </c>
+      <c r="C37" t="str">
+        <v>two_layer_lstm</v>
+      </c>
+      <c r="D37">
+        <v>1E-4</v>
+      </c>
+      <c r="E37">
+        <v>1.6925195889746902E-2</v>
+      </c>
+      <c r="F37">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B38">
+        <v>35</v>
+      </c>
+      <c r="C38" t="str">
+        <v>two_layer_lstm</v>
+      </c>
+      <c r="D38">
+        <v>1E-4</v>
+      </c>
+      <c r="E38">
+        <v>1.7261049261437698E-2</v>
+      </c>
+      <c r="F38">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B39">
+        <v>36</v>
+      </c>
+      <c r="C39" t="str">
+        <v>lstm_with_dropout</v>
+      </c>
+      <c r="D39">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E39">
+        <v>1.3072971143280199E-2</v>
+      </c>
+      <c r="F39">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B40">
+        <v>37</v>
+      </c>
+      <c r="C40" t="str">
+        <v>lstm_with_dropout</v>
+      </c>
+      <c r="D40">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E40">
+        <v>1.3409412447017001E-2</v>
+      </c>
+      <c r="F40">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B41">
+        <v>38</v>
+      </c>
+      <c r="C41" t="str">
+        <v>lstm_with_dropout</v>
+      </c>
+      <c r="D41">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E41">
+        <v>1.31754729189121E-2</v>
+      </c>
+      <c r="F41">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B42">
+        <v>39</v>
+      </c>
+      <c r="C42" t="str">
+        <v>lstm_with_dropout</v>
+      </c>
+      <c r="D42">
+        <v>1E-3</v>
+      </c>
+      <c r="E42">
+        <v>1.37466485769197E-2</v>
+      </c>
+      <c r="F42">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B43">
+        <v>40</v>
+      </c>
+      <c r="C43" t="str">
+        <v>lstm_with_dropout</v>
+      </c>
+      <c r="D43">
+        <v>1E-3</v>
+      </c>
+      <c r="E43">
+        <v>1.43648884077758E-2</v>
+      </c>
+      <c r="F43">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B44">
+        <v>41</v>
+      </c>
+      <c r="C44" t="str">
+        <v>lstm_with_dropout</v>
+      </c>
+      <c r="D44">
+        <v>1E-3</v>
+      </c>
+      <c r="E44">
+        <v>1.4029454769513601E-2</v>
+      </c>
+      <c r="F44">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B45">
+        <v>42</v>
+      </c>
+      <c r="C45" t="str">
+        <v>lstm_with_dropout</v>
+      </c>
+      <c r="D45">
+        <v>1E-4</v>
+      </c>
+      <c r="E45">
+        <v>3.0069533092561E-2</v>
+      </c>
+      <c r="F45">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B46">
+        <v>43</v>
+      </c>
+      <c r="C46" t="str">
+        <v>lstm_with_dropout</v>
+      </c>
+      <c r="D46">
+        <v>1E-4</v>
+      </c>
+      <c r="E46">
+        <v>1.9186440916604399E-2</v>
+      </c>
+      <c r="F46">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B47">
+        <v>44</v>
+      </c>
+      <c r="C47" t="str">
+        <v>lstm_with_dropout</v>
+      </c>
+      <c r="D47">
+        <v>1E-4</v>
+      </c>
+      <c r="E47">
+        <v>1.8438776518417001E-2</v>
+      </c>
+      <c r="F47">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B48">
+        <v>45</v>
+      </c>
+      <c r="C48" t="str">
+        <v>bidirectional_lstm</v>
+      </c>
+      <c r="D48">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E48">
+        <v>1.27822315974778E-2</v>
+      </c>
+      <c r="F48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B49">
+        <v>46</v>
+      </c>
+      <c r="C49" t="str">
+        <v>bidirectional_lstm</v>
+      </c>
+      <c r="D49">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E49">
+        <v>1.2810149757597301E-2</v>
+      </c>
+      <c r="F49">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B50">
+        <v>47</v>
+      </c>
+      <c r="C50" t="str">
+        <v>bidirectional_lstm</v>
+      </c>
+      <c r="D50">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E50">
+        <v>1.26819633451235E-2</v>
+      </c>
+      <c r="F50">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B51">
+        <v>48</v>
+      </c>
+      <c r="C51" t="str">
+        <v>bidirectional_lstm</v>
+      </c>
+      <c r="D51">
+        <v>1E-3</v>
+      </c>
+      <c r="E51">
+        <v>1.3357209280299299E-2</v>
+      </c>
+      <c r="F51">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B52">
+        <v>49</v>
+      </c>
+      <c r="C52" t="str">
+        <v>bidirectional_lstm</v>
+      </c>
+      <c r="D52">
+        <v>1E-3</v>
+      </c>
+      <c r="E52">
+        <v>1.3467765253163601E-2</v>
+      </c>
+      <c r="F52">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B53">
+        <v>50</v>
+      </c>
+      <c r="C53" t="str">
+        <v>bidirectional_lstm</v>
+      </c>
+      <c r="D53">
+        <v>1E-3</v>
+      </c>
+      <c r="E53">
+        <v>1.3160275507805999E-2</v>
+      </c>
+      <c r="F53">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B54">
+        <v>51</v>
+      </c>
+      <c r="C54" t="str">
+        <v>bidirectional_lstm</v>
+      </c>
+      <c r="D54">
+        <v>1E-4</v>
+      </c>
+      <c r="E54">
+        <v>2.0527414071028101E-2</v>
+      </c>
+      <c r="F54">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B55">
+        <v>52</v>
+      </c>
+      <c r="C55" t="str">
+        <v>bidirectional_lstm</v>
+      </c>
+      <c r="D55">
+        <v>1E-4</v>
+      </c>
+      <c r="E55">
+        <v>1.7148232968310698E-2</v>
+      </c>
+      <c r="F55">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B56">
+        <v>53</v>
+      </c>
+      <c r="C56" t="str">
+        <v>bidirectional_lstm</v>
+      </c>
+      <c r="D56">
+        <v>1E-4</v>
+      </c>
+      <c r="E56">
+        <v>1.5869693635132E-2</v>
+      </c>
+      <c r="F56">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B57">
+        <v>54</v>
+      </c>
+      <c r="C57" t="str">
+        <v>lstm_with_recurrent_dropout</v>
+      </c>
+      <c r="D57">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E57">
+        <v>1.22920567428916E-2</v>
+      </c>
+      <c r="F57">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B58">
+        <v>55</v>
+      </c>
+      <c r="C58" t="str">
+        <v>lstm_with_recurrent_dropout</v>
+      </c>
+      <c r="D58">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E58">
+        <v>1.23273342059064E-2</v>
+      </c>
+      <c r="F58">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B59">
+        <v>56</v>
+      </c>
+      <c r="C59" t="str">
+        <v>lstm_with_recurrent_dropout</v>
+      </c>
+      <c r="D59">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E59">
+        <v>1.21777261257507E-2</v>
+      </c>
+      <c r="F59">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B60">
+        <v>57</v>
+      </c>
+      <c r="C60" t="str">
+        <v>lstm_with_recurrent_dropout</v>
+      </c>
+      <c r="D60">
+        <v>1E-3</v>
+      </c>
+      <c r="E60">
+        <v>1.4564609630136E-2</v>
+      </c>
+      <c r="F60">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B61">
+        <v>58</v>
+      </c>
+      <c r="C61" t="str">
+        <v>lstm_with_recurrent_dropout</v>
+      </c>
+      <c r="D61">
+        <v>1E-3</v>
+      </c>
+      <c r="E61">
+        <v>1.44525050055259E-2</v>
+      </c>
+      <c r="F61">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B62">
+        <v>59</v>
+      </c>
+      <c r="C62" t="str">
+        <v>lstm_with_recurrent_dropout</v>
+      </c>
+      <c r="D62">
+        <v>1E-3</v>
+      </c>
+      <c r="E62">
+        <v>1.3982253469699E-2</v>
+      </c>
+      <c r="F62">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="63" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B63">
+        <v>60</v>
+      </c>
+      <c r="C63" t="str">
+        <v>lstm_with_recurrent_dropout</v>
+      </c>
+      <c r="D63">
+        <v>1E-4</v>
+      </c>
+      <c r="E63">
+        <v>2.6357614833328099E-2</v>
+      </c>
+      <c r="F63">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="64" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B64">
+        <v>61</v>
+      </c>
+      <c r="C64" t="str">
+        <v>lstm_with_recurrent_dropout</v>
+      </c>
+      <c r="D64">
+        <v>1E-4</v>
+      </c>
+      <c r="E64">
+        <v>2.1192315397628801E-2</v>
+      </c>
+      <c r="F64">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="65" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B65">
+        <v>62</v>
+      </c>
+      <c r="C65" t="str">
+        <v>lstm_with_recurrent_dropout</v>
+      </c>
+      <c r="D65">
+        <v>1E-4</v>
+      </c>
+      <c r="E65">
+        <v>1.8319126836407601E-2</v>
+      </c>
+      <c r="F65">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="66" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B66">
+        <v>63</v>
+      </c>
+      <c r="C66" t="str">
+        <v>deep_lstm_with_dense_layers</v>
+      </c>
+      <c r="D66">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E66">
+        <v>1.45938925706341E-2</v>
+      </c>
+      <c r="F66">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="67" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B67">
+        <v>64</v>
+      </c>
+      <c r="C67" t="str">
+        <v>deep_lstm_with_dense_layers</v>
+      </c>
+      <c r="D67">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E67">
+        <v>1.3085099663377999E-2</v>
+      </c>
+      <c r="F67">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="68" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B68">
+        <v>65</v>
+      </c>
+      <c r="C68" t="str">
+        <v>deep_lstm_with_dense_layers</v>
+      </c>
+      <c r="D68">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E68">
+        <v>1.2814309800628899E-2</v>
+      </c>
+      <c r="F68">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="69" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B69">
+        <v>66</v>
+      </c>
+      <c r="C69" t="str">
+        <v>deep_lstm_with_dense_layers</v>
+      </c>
+      <c r="D69">
+        <v>1E-3</v>
+      </c>
+      <c r="E69">
+        <v>1.44374926040053E-2</v>
+      </c>
+      <c r="F69">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="70" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B70">
+        <v>67</v>
+      </c>
+      <c r="C70" t="str">
+        <v>deep_lstm_with_dense_layers</v>
+      </c>
+      <c r="D70">
+        <v>1E-3</v>
+      </c>
+      <c r="E70">
+        <v>1.3926222644110401E-2</v>
+      </c>
+      <c r="F70">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="71" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B71">
+        <v>68</v>
+      </c>
+      <c r="C71" t="str">
+        <v>deep_lstm_with_dense_layers</v>
+      </c>
+      <c r="D71">
+        <v>1E-3</v>
+      </c>
+      <c r="E71">
+        <v>1.3208990878852399E-2</v>
+      </c>
+      <c r="F71">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B72">
+        <v>69</v>
+      </c>
+      <c r="C72" t="str">
+        <v>deep_lstm_with_dense_layers</v>
+      </c>
+      <c r="D72">
+        <v>1E-4</v>
+      </c>
+      <c r="E72">
+        <v>3.52212050266646E-2</v>
+      </c>
+      <c r="F72">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="73" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B73">
+        <v>70</v>
+      </c>
+      <c r="C73" t="str">
+        <v>deep_lstm_with_dense_layers</v>
+      </c>
+      <c r="D73">
+        <v>1E-4</v>
+      </c>
+      <c r="E73">
+        <v>2.9589054774021E-2</v>
+      </c>
+      <c r="F73">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="74" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B74">
+        <v>71</v>
+      </c>
+      <c r="C74" t="str">
+        <v>deep_lstm_with_dense_layers</v>
+      </c>
+      <c r="D74">
+        <v>1E-4</v>
+      </c>
+      <c r="E74">
+        <v>1.6287797107392001E-2</v>
+      </c>
+      <c r="F74">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="75" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B75">
+        <v>72</v>
+      </c>
+      <c r="C75" t="str">
+        <v>cnn_lstm_hybrid</v>
+      </c>
+      <c r="D75">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E75">
+        <v>1.43905322851554E-2</v>
+      </c>
+      <c r="F75">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="76" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B76">
+        <v>73</v>
+      </c>
+      <c r="C76" t="str">
+        <v>cnn_lstm_hybrid</v>
+      </c>
+      <c r="D76">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E76">
+        <v>1.4350034196295399E-2</v>
+      </c>
+      <c r="F76">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="77" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B77">
+        <v>74</v>
+      </c>
+      <c r="C77" t="str">
+        <v>cnn_lstm_hybrid</v>
+      </c>
+      <c r="D77">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E77">
+        <v>1.37627288611014E-2</v>
+      </c>
+      <c r="F77">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="78" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B78">
+        <v>75</v>
+      </c>
+      <c r="C78" t="str">
+        <v>cnn_lstm_hybrid</v>
+      </c>
+      <c r="D78">
+        <v>1E-3</v>
+      </c>
+      <c r="E78">
+        <v>1.6574639351044199E-2</v>
+      </c>
+      <c r="F78">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="79" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B79">
+        <v>76</v>
+      </c>
+      <c r="C79" t="str">
+        <v>cnn_lstm_hybrid</v>
+      </c>
+      <c r="D79">
+        <v>1E-3</v>
+      </c>
+      <c r="E79">
+        <v>1.64955460021445E-2</v>
+      </c>
+      <c r="F79">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="80" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B80">
+        <v>77</v>
+      </c>
+      <c r="C80" t="str">
+        <v>cnn_lstm_hybrid</v>
+      </c>
+      <c r="D80">
+        <v>1E-3</v>
+      </c>
+      <c r="E80">
+        <v>1.46397206251662E-2</v>
+      </c>
+      <c r="F80">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B81">
+        <v>78</v>
+      </c>
+      <c r="C81" t="str">
+        <v>cnn_lstm_hybrid</v>
+      </c>
+      <c r="D81">
+        <v>1E-4</v>
+      </c>
+      <c r="E81">
+        <v>4.2551470863707697E-2</v>
+      </c>
+      <c r="F81">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B82">
+        <v>79</v>
+      </c>
+      <c r="C82" t="str">
+        <v>cnn_lstm_hybrid</v>
+      </c>
+      <c r="D82">
+        <v>1E-4</v>
+      </c>
+      <c r="E82">
+        <v>1.9215282779771099E-2</v>
+      </c>
+      <c r="F82">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B83">
+        <v>80</v>
+      </c>
+      <c r="C83" t="str">
+        <v>cnn_lstm_hybrid</v>
+      </c>
+      <c r="D83">
+        <v>1E-4</v>
+      </c>
+      <c r="E83">
+        <v>2.0641193830808299E-2</v>
+      </c>
+      <c r="F83">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B84">
+        <v>81</v>
+      </c>
+      <c r="C84" t="str">
+        <v>shallow_lstm_linear_output</v>
+      </c>
+      <c r="D84">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E84">
+        <v>1.28265260079588E-2</v>
+      </c>
+      <c r="F84">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="85" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B85">
+        <v>82</v>
+      </c>
+      <c r="C85" t="str">
+        <v>shallow_lstm_linear_output</v>
+      </c>
+      <c r="D85">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E85">
+        <v>1.16570501701606E-2</v>
+      </c>
+      <c r="F85">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B86">
+        <v>83</v>
+      </c>
+      <c r="C86" t="str">
+        <v>shallow_lstm_linear_output</v>
+      </c>
+      <c r="D86">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E86">
+        <v>1.22438158214611E-2</v>
+      </c>
+      <c r="F86">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="87" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B87">
+        <v>84</v>
+      </c>
+      <c r="C87" t="str">
+        <v>shallow_lstm_linear_output</v>
+      </c>
+      <c r="D87">
+        <v>1E-3</v>
+      </c>
+      <c r="E87">
+        <v>1.49863818067065E-2</v>
+      </c>
+      <c r="F87">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="88" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B88">
+        <v>85</v>
+      </c>
+      <c r="C88" t="str">
+        <v>shallow_lstm_linear_output</v>
+      </c>
+      <c r="D88">
+        <v>1E-3</v>
+      </c>
+      <c r="E88">
+        <v>1.4492875495398501E-2</v>
+      </c>
+      <c r="F88">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="89" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B89">
+        <v>86</v>
+      </c>
+      <c r="C89" t="str">
+        <v>shallow_lstm_linear_output</v>
+      </c>
+      <c r="D89">
+        <v>1E-3</v>
+      </c>
+      <c r="E89">
+        <v>1.4334032449032801E-2</v>
+      </c>
+      <c r="F89">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="90" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B90">
+        <v>87</v>
+      </c>
+      <c r="C90" t="str">
+        <v>shallow_lstm_linear_output</v>
+      </c>
+      <c r="D90">
+        <v>1E-4</v>
+      </c>
+      <c r="E90">
+        <v>7.1023261470411894E-2</v>
+      </c>
+      <c r="F90">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="91" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B91">
+        <v>88</v>
+      </c>
+      <c r="C91" t="str">
+        <v>shallow_lstm_linear_output</v>
+      </c>
+      <c r="D91">
+        <v>1E-4</v>
+      </c>
+      <c r="E91">
+        <v>5.61272497063268E-2</v>
+      </c>
+      <c r="F91">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="92" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B92">
+        <v>89</v>
+      </c>
+      <c r="C92" t="str">
+        <v>shallow_lstm_linear_output</v>
+      </c>
+      <c r="D92">
+        <v>1E-4</v>
+      </c>
+      <c r="E92">
+        <v>2.5267449207353399E-2</v>
+      </c>
+      <c r="F92">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="93" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B93">
+        <v>90</v>
+      </c>
+      <c r="C93" t="str">
+        <v>two_layer_bidirectional_lstm</v>
+      </c>
+      <c r="D93">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E93">
+        <v>1.44023132514394E-2</v>
+      </c>
+      <c r="F93">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="94" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B94">
+        <v>91</v>
+      </c>
+      <c r="C94" t="str">
+        <v>two_layer_bidirectional_lstm</v>
+      </c>
+      <c r="D94">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E94">
+        <v>1.23456500354879E-2</v>
+      </c>
+      <c r="F94">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="95" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B95">
+        <v>92</v>
+      </c>
+      <c r="C95" t="str">
+        <v>two_layer_bidirectional_lstm</v>
+      </c>
+      <c r="D95">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E95">
+        <v>1.50261211549225E-2</v>
+      </c>
+      <c r="F95">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="96" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B96">
+        <v>93</v>
+      </c>
+      <c r="C96" t="str">
+        <v>two_layer_bidirectional_lstm</v>
+      </c>
+      <c r="D96">
+        <v>1E-3</v>
+      </c>
+      <c r="E96">
+        <v>1.31539659195267E-2</v>
+      </c>
+      <c r="F96">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="97" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B97">
+        <v>94</v>
+      </c>
+      <c r="C97" t="str">
+        <v>two_layer_bidirectional_lstm</v>
+      </c>
+      <c r="D97">
+        <v>1E-3</v>
+      </c>
+      <c r="E97">
+        <v>1.2685153271395E-2</v>
+      </c>
+      <c r="F97">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="98" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B98">
+        <v>95</v>
+      </c>
+      <c r="C98" t="str">
+        <v>two_layer_bidirectional_lstm</v>
+      </c>
+      <c r="D98">
+        <v>1E-3</v>
+      </c>
+      <c r="E98">
+        <v>1.3205394607113801E-2</v>
+      </c>
+      <c r="F98">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="99" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B99">
+        <v>96</v>
+      </c>
+      <c r="C99" t="str">
+        <v>two_layer_bidirectional_lstm</v>
+      </c>
+      <c r="D99">
+        <v>1E-4</v>
+      </c>
+      <c r="E99">
+        <v>1.6928615226145902E-2</v>
+      </c>
+      <c r="F99">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="100" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B100">
+        <v>97</v>
+      </c>
+      <c r="C100" t="str">
+        <v>two_layer_bidirectional_lstm</v>
+      </c>
+      <c r="D100">
+        <v>1E-4</v>
+      </c>
+      <c r="E100">
+        <v>1.6247783802011601E-2</v>
+      </c>
+      <c r="F100">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="101" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B101">
+        <v>98</v>
+      </c>
+      <c r="C101" t="str">
+        <v>two_layer_bidirectional_lstm</v>
+      </c>
+      <c r="D101">
+        <v>1E-4</v>
+      </c>
+      <c r="E101">
+        <v>1.57259552290064E-2</v>
+      </c>
+      <c r="F101">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="102" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B102">
+        <v>99</v>
+      </c>
+      <c r="C102" t="str">
+        <v>deep_bidirectional_lstm_with_dropout</v>
+      </c>
+      <c r="D102">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E102">
+        <v>1.36001363928831E-2</v>
+      </c>
+      <c r="F102">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="103" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B103">
+        <v>100</v>
+      </c>
+      <c r="C103" t="str">
+        <v>deep_bidirectional_lstm_with_dropout</v>
+      </c>
+      <c r="D103">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E103">
+        <v>1.26807558799093E-2</v>
+      </c>
+      <c r="F103">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="104" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B104">
+        <v>101</v>
+      </c>
+      <c r="C104" t="str">
+        <v>deep_bidirectional_lstm_with_dropout</v>
+      </c>
+      <c r="D104">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E104">
+        <v>1.25949114305711E-2</v>
+      </c>
+      <c r="F104">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="105" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B105">
+        <v>102</v>
+      </c>
+      <c r="C105" t="str">
+        <v>deep_bidirectional_lstm_with_dropout</v>
+      </c>
+      <c r="D105">
+        <v>1E-3</v>
+      </c>
+      <c r="E105">
+        <v>1.29735103709963E-2</v>
+      </c>
+      <c r="F105">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="106" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B106">
+        <v>103</v>
+      </c>
+      <c r="C106" t="str">
+        <v>deep_bidirectional_lstm_with_dropout</v>
+      </c>
+      <c r="D106">
+        <v>1E-3</v>
+      </c>
+      <c r="E106">
+        <v>1.2574239980512599E-2</v>
+      </c>
+      <c r="F106">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="107" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B107">
+        <v>104</v>
+      </c>
+      <c r="C107" t="str">
+        <v>deep_bidirectional_lstm_with_dropout</v>
+      </c>
+      <c r="D107">
+        <v>1E-3</v>
+      </c>
+      <c r="E107">
+        <v>1.2838059811580701E-2</v>
+      </c>
+      <c r="F107">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="108" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B108">
+        <v>105</v>
+      </c>
+      <c r="C108" t="str">
+        <v>deep_bidirectional_lstm_with_dropout</v>
+      </c>
+      <c r="D108">
+        <v>1E-4</v>
+      </c>
+      <c r="E108">
+        <v>1.6649904743909899E-2</v>
+      </c>
+      <c r="F108">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="109" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B109">
+        <v>106</v>
+      </c>
+      <c r="C109" t="str">
+        <v>deep_bidirectional_lstm_with_dropout</v>
+      </c>
+      <c r="D109">
+        <v>1E-4</v>
+      </c>
+      <c r="E109">
+        <v>1.5615455539398001E-2</v>
+      </c>
+      <c r="F109">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="110" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B110">
+        <v>107</v>
+      </c>
+      <c r="C110" t="str">
+        <v>deep_bidirectional_lstm_with_dropout</v>
+      </c>
+      <c r="D110">
+        <v>1E-4</v>
+      </c>
+      <c r="E110">
+        <v>1.4201131491095999E-2</v>
+      </c>
+      <c r="F110">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="111" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B111">
+        <v>108</v>
+      </c>
+      <c r="C111" t="str">
+        <v>bidirectional_lstm_with_dense_layers</v>
+      </c>
+      <c r="D111">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E111">
+        <v>1.3265948631743E-2</v>
+      </c>
+      <c r="F111">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="112" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B112">
+        <v>109</v>
+      </c>
+      <c r="C112" t="str">
+        <v>bidirectional_lstm_with_dense_layers</v>
+      </c>
+      <c r="D112">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E112">
+        <v>1.3309568909900199E-2</v>
+      </c>
+      <c r="F112">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="113" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B113">
+        <v>110</v>
+      </c>
+      <c r="C113" t="str">
+        <v>bidirectional_lstm_with_dense_layers</v>
+      </c>
+      <c r="D113">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E113">
+        <v>1.3508142449827299E-2</v>
+      </c>
+      <c r="F113">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="114" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B114">
+        <v>111</v>
+      </c>
+      <c r="C114" t="str">
+        <v>bidirectional_lstm_with_dense_layers</v>
+      </c>
+      <c r="D114">
+        <v>1E-3</v>
+      </c>
+      <c r="E114">
+        <v>1.36025925676344E-2</v>
+      </c>
+      <c r="F114">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="115" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B115">
+        <v>112</v>
+      </c>
+      <c r="C115" t="str">
+        <v>bidirectional_lstm_with_dense_layers</v>
+      </c>
+      <c r="D115">
+        <v>1E-3</v>
+      </c>
+      <c r="E115">
+        <v>1.3197067170436E-2</v>
+      </c>
+      <c r="F115">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="116" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B116">
+        <v>113</v>
+      </c>
+      <c r="C116" t="str">
+        <v>bidirectional_lstm_with_dense_layers</v>
+      </c>
+      <c r="D116">
+        <v>1E-3</v>
+      </c>
+      <c r="E116">
+        <v>1.31288622589395E-2</v>
+      </c>
+      <c r="F116">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="117" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B117">
+        <v>114</v>
+      </c>
+      <c r="C117" t="str">
+        <v>bidirectional_lstm_with_dense_layers</v>
+      </c>
+      <c r="D117">
+        <v>1E-4</v>
+      </c>
+      <c r="E117">
+        <v>1.64048683027005E-2</v>
+      </c>
+      <c r="F117">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="118" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B118">
+        <v>115</v>
+      </c>
+      <c r="C118" t="str">
+        <v>bidirectional_lstm_with_dense_layers</v>
+      </c>
+      <c r="D118">
+        <v>1E-4</v>
+      </c>
+      <c r="E118">
+        <v>1.5451870911122901E-2</v>
+      </c>
+      <c r="F118">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="119" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B119">
+        <v>116</v>
+      </c>
+      <c r="C119" t="str">
+        <v>bidirectional_lstm_with_dense_layers</v>
+      </c>
+      <c r="D119">
+        <v>1E-4</v>
+      </c>
+      <c r="E119">
+        <v>1.45336655471446E-2</v>
+      </c>
+      <c r="F119">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="120" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B120">
+        <v>117</v>
+      </c>
+      <c r="C120" t="str">
+        <v>cnn_bidirectional_lstm_hybrid</v>
+      </c>
+      <c r="D120">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E120">
+        <v>1.4410346819826199E-2</v>
+      </c>
+      <c r="F120">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="121" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B121">
+        <v>118</v>
+      </c>
+      <c r="C121" t="str">
+        <v>cnn_bidirectional_lstm_hybrid</v>
+      </c>
+      <c r="D121">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E121">
+        <v>1.38359638701058E-2</v>
+      </c>
+      <c r="F121">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="122" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B122">
+        <v>119</v>
+      </c>
+      <c r="C122" t="str">
+        <v>cnn_bidirectional_lstm_hybrid</v>
+      </c>
+      <c r="D122">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E122">
+        <v>1.31175909608415E-2</v>
+      </c>
+      <c r="F122">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="123" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B123">
+        <v>120</v>
+      </c>
+      <c r="C123" t="str">
+        <v>cnn_bidirectional_lstm_hybrid</v>
+      </c>
+      <c r="D123">
+        <v>1E-3</v>
+      </c>
+      <c r="E123">
+        <v>1.5730358232924999E-2</v>
+      </c>
+      <c r="F123">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="124" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B124">
+        <v>121</v>
+      </c>
+      <c r="C124" t="str">
+        <v>cnn_bidirectional_lstm_hybrid</v>
+      </c>
+      <c r="D124">
+        <v>1E-3</v>
+      </c>
+      <c r="E124">
+        <v>1.52824542617968E-2</v>
+      </c>
+      <c r="F124">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="125" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B125">
+        <v>122</v>
+      </c>
+      <c r="C125" t="str">
+        <v>cnn_bidirectional_lstm_hybrid</v>
+      </c>
+      <c r="D125">
+        <v>1E-3</v>
+      </c>
+      <c r="E125">
+        <v>1.4404213538010999E-2</v>
+      </c>
+      <c r="F125">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="126" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B126">
+        <v>123</v>
+      </c>
+      <c r="C126" t="str">
+        <v>cnn_bidirectional_lstm_hybrid</v>
+      </c>
+      <c r="D126">
+        <v>1E-4</v>
+      </c>
+      <c r="E126">
+        <v>1.6992096129641501E-2</v>
+      </c>
+      <c r="F126">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="127" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B127">
+        <v>124</v>
+      </c>
+      <c r="C127" t="str">
+        <v>cnn_bidirectional_lstm_hybrid</v>
+      </c>
+      <c r="D127">
+        <v>1E-4</v>
+      </c>
+      <c r="E127">
+        <v>1.7696928875926499E-2</v>
+      </c>
+      <c r="F127">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="128" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B128">
+        <v>125</v>
+      </c>
+      <c r="C128" t="str">
+        <v>cnn_bidirectional_lstm_hybrid</v>
+      </c>
+      <c r="D128">
+        <v>1E-4</v>
+      </c>
+      <c r="E128">
+        <v>1.7066252927506999E-2</v>
+      </c>
+      <c r="F128">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="129" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B129">
+        <v>126</v>
+      </c>
+      <c r="C129" t="str">
+        <v>very_deep_bidirectional_lstm</v>
+      </c>
+      <c r="D129">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E129">
+        <v>1.22961265051606E-2</v>
+      </c>
+      <c r="F129">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="130" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B130">
+        <v>127</v>
+      </c>
+      <c r="C130" t="str">
+        <v>very_deep_bidirectional_lstm</v>
+      </c>
+      <c r="D130">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E130">
+        <v>1.24594107411865E-2</v>
+      </c>
+      <c r="F130">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="131" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B131">
+        <v>128</v>
+      </c>
+      <c r="C131" t="str">
+        <v>very_deep_bidirectional_lstm</v>
+      </c>
+      <c r="D131">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E131">
+        <v>1.20864642114687E-2</v>
+      </c>
+      <c r="F131">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="132" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B132">
+        <v>129</v>
+      </c>
+      <c r="C132" t="str">
+        <v>very_deep_bidirectional_lstm</v>
+      </c>
+      <c r="D132">
+        <v>1E-3</v>
+      </c>
+      <c r="E132">
+        <v>1.2669296201962299E-2</v>
+      </c>
+      <c r="F132">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="133" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B133">
+        <v>130</v>
+      </c>
+      <c r="C133" t="str">
+        <v>very_deep_bidirectional_lstm</v>
+      </c>
+      <c r="D133">
+        <v>1E-3</v>
+      </c>
+      <c r="E133">
+        <v>1.2723149812480201E-2</v>
+      </c>
+      <c r="F133">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="134" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B134">
+        <v>131</v>
+      </c>
+      <c r="C134" t="str">
+        <v>very_deep_bidirectional_lstm</v>
+      </c>
+      <c r="D134">
+        <v>1E-3</v>
+      </c>
+      <c r="E134">
+        <v>1.29642609066817E-2</v>
+      </c>
+      <c r="F134">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="135" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B135">
+        <v>132</v>
+      </c>
+      <c r="C135" t="str">
+        <v>very_deep_bidirectional_lstm</v>
+      </c>
+      <c r="D135">
+        <v>1E-4</v>
+      </c>
+      <c r="E135">
+        <v>1.4791897743051299E-2</v>
+      </c>
+      <c r="F135">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="136" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B136">
+        <v>133</v>
+      </c>
+      <c r="C136" t="str">
+        <v>very_deep_bidirectional_lstm</v>
+      </c>
+      <c r="D136">
+        <v>1E-4</v>
+      </c>
+      <c r="E136">
+        <v>1.4494184892627699E-2</v>
+      </c>
+      <c r="F136">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="137" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B137">
+        <v>134</v>
+      </c>
+      <c r="C137" t="str">
+        <v>very_deep_bidirectional_lstm</v>
+      </c>
+      <c r="D137">
+        <v>1E-4</v>
+      </c>
+      <c r="E137">
+        <v>1.3756304283510001E-2</v>
+      </c>
+      <c r="F137">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="138" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B138">
+        <v>135</v>
+      </c>
+      <c r="C138" t="str">
+        <v>bidirectional_lstm_with_batch_norm</v>
+      </c>
+      <c r="D138">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E138">
+        <v>2.3268492313405699E-2</v>
+      </c>
+      <c r="F138">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="139" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B139">
+        <v>136</v>
+      </c>
+      <c r="C139" t="str">
+        <v>bidirectional_lstm_with_batch_norm</v>
+      </c>
+      <c r="D139">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E139">
+        <v>1.6152695640086999E-2</v>
+      </c>
+      <c r="F139">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="140" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B140">
+        <v>137</v>
+      </c>
+      <c r="C140" t="str">
+        <v>bidirectional_lstm_with_batch_norm</v>
+      </c>
+      <c r="D140">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="E140">
+        <v>1.9238502156269498E-2</v>
+      </c>
+      <c r="F140">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B141">
+        <v>138</v>
+      </c>
+      <c r="C141" t="str">
+        <v>bidirectional_lstm_with_batch_norm</v>
+      </c>
+      <c r="D141">
+        <v>1E-3</v>
+      </c>
+      <c r="E141">
+        <v>0.17610738919458299</v>
+      </c>
+      <c r="F141">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="142" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B142">
+        <v>139</v>
+      </c>
+      <c r="C142" t="str">
+        <v>bidirectional_lstm_with_batch_norm</v>
+      </c>
+      <c r="D142">
+        <v>1E-3</v>
+      </c>
+      <c r="E142">
+        <v>0.15086367288616201</v>
+      </c>
+      <c r="F142">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="143" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B143">
+        <v>140</v>
+      </c>
+      <c r="C143" t="str">
+        <v>bidirectional_lstm_with_batch_norm</v>
+      </c>
+      <c r="D143">
+        <v>1E-3</v>
+      </c>
+      <c r="E143">
+        <v>0.11950052459305301</v>
+      </c>
+      <c r="F143">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="144" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B144">
+        <v>141</v>
+      </c>
+      <c r="C144" t="str">
+        <v>bidirectional_lstm_with_batch_norm</v>
+      </c>
+      <c r="D144">
+        <v>1E-4</v>
+      </c>
+      <c r="E144">
+        <v>0.19860009013004301</v>
+      </c>
+      <c r="F144">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="145" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B145">
+        <v>142</v>
+      </c>
+      <c r="C145" t="str">
+        <v>bidirectional_lstm_with_batch_norm</v>
+      </c>
+      <c r="D145">
+        <v>1E-4</v>
+      </c>
+      <c r="E145">
+        <v>0.12898558897690601</v>
+      </c>
+      <c r="F145">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="146" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B146">
+        <v>143</v>
+      </c>
+      <c r="C146" t="str">
+        <v>bidirectional_lstm_with_batch_norm</v>
+      </c>
+      <c r="D146">
+        <v>1E-4</v>
+      </c>
+      <c r="E146">
+        <v>0.15354245579492001</v>
+      </c>
+      <c r="F146">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>